<commit_message>
finished determining MMOI experimentally
</commit_message>
<xml_diff>
--- a/Barrowman(1.04).xlsx
+++ b/Barrowman(1.04).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bktf3\Desktop\rocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3649606D-18DC-4D7D-B518-20DE6BF6D21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE43215-2481-4CBC-A30E-76040BA02933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1740" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7140" yWindow="3450" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="6" r:id="rId1"/>
@@ -7695,8 +7695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8098,7 +8098,7 @@
       <c r="L23" s="61"/>
       <c r="M23" s="61"/>
       <c r="N23" s="13">
-        <v>40</v>
+        <v>41.5</v>
       </c>
       <c r="O23" s="61"/>
       <c r="P23" s="62"/>
@@ -8160,7 +8160,7 @@
       <c r="K27" s="61"/>
       <c r="L27" s="61"/>
       <c r="M27" s="13">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N27" s="61"/>
       <c r="O27" s="61"/>
@@ -8176,7 +8176,7 @@
       <c r="L28" s="61"/>
       <c r="M28" s="61"/>
       <c r="N28" s="14">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="O28" s="61"/>
       <c r="P28" s="62"/>
@@ -8218,8 +8218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="D28" s="53">
         <f>Figure!N28</f>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>5</v>
@@ -8824,7 +8824,7 @@
       </c>
       <c r="D31" s="28">
         <f>IF(D25="yes",xpb+ltb/3*(1+(1-dfb/drb)/(1-(dfb/drb)^2)),0)</f>
-        <v>740.84615384615381</v>
+        <v>741.08974358974353</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>5</v>
@@ -8956,7 +8956,7 @@
       </c>
       <c r="D38" s="53">
         <f>Figure!M27</f>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E38" s="17" t="s">
         <v>5</v>
@@ -8976,7 +8976,7 @@
       </c>
       <c r="D39" s="53">
         <f>Figure!N23</f>
-        <v>40</v>
+        <v>41.5</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>5</v>
@@ -9075,7 +9075,7 @@
       </c>
       <c r="D44" s="32">
         <f>(1+rad/(s+rad))*4*n*(s/dia)^2/(1+SQRT(1+(2*lf/(cr+ct))^2))</f>
-        <v>15.376368517885188</v>
+        <v>15.151726563717666</v>
       </c>
       <c r="E44" s="70" t="s">
         <v>135</v>
@@ -9097,7 +9097,7 @@
       </c>
       <c r="D45" s="28">
         <f>xb+xr*(cr+2*ct)/3/(cr+ct)+1/6*((cr+ct)-cr*ct/(cr+ct))</f>
-        <v>708.97058823529403</v>
+        <v>709.03658536585363</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>5</v>
@@ -9132,7 +9132,7 @@
       </c>
       <c r="D47" s="41">
         <f>cnn+cnf+cnt+cntb</f>
-        <v>16.845756272987231</v>
+        <v>16.621114318819707</v>
       </c>
       <c r="E47" s="42"/>
       <c r="F47" s="43" t="s">
@@ -9152,7 +9152,7 @@
       </c>
       <c r="D48" s="47">
         <f>(cnn*xn+cnt*xt+cntb*xtb+cnf*xf)/cnr</f>
-        <v>627.11408268273954</v>
+        <v>626.06014091583484</v>
       </c>
       <c r="E48" s="48" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
incorrect nose cone length measurement. changed 0.06 m to 0.16 m and recalculated Cp to 0.626 to 0.632
</commit_message>
<xml_diff>
--- a/Barrowman(1.04).xlsx
+++ b/Barrowman(1.04).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bktf3\Desktop\rocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE43215-2481-4CBC-A30E-76040BA02933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F45170-B215-4D1B-ADBB-16F1A46BFF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="3450" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="6" r:id="rId1"/>
@@ -71,6 +71,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -7696,7 +7699,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7755,7 +7758,7 @@
       <c r="H5" s="59"/>
       <c r="I5" s="60"/>
       <c r="J5" s="11">
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="K5" s="60"/>
       <c r="L5" s="60"/>
@@ -8218,8 +8221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8370,7 +8373,7 @@
       </c>
       <c r="D9" s="53">
         <f>Figure!J5</f>
-        <v>60</v>
+        <v>160</v>
       </c>
       <c r="E9" s="26" t="s">
         <v>5</v>
@@ -8464,7 +8467,7 @@
       </c>
       <c r="D13" s="28">
         <f>D12*ln</f>
-        <v>27.96</v>
+        <v>74.56</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>5</v>
@@ -9152,7 +9155,7 @@
       </c>
       <c r="D48" s="47">
         <f>(cnn*xn+cnt*xt+cntb*xtb+cnf*xf)/cnr</f>
-        <v>626.06014091583484</v>
+        <v>631.66746652663767</v>
       </c>
       <c r="E48" s="48" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
corrected Cl coefficient from 16.85 to 16.62
</commit_message>
<xml_diff>
--- a/Barrowman(1.04).xlsx
+++ b/Barrowman(1.04).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bktf3\Desktop\rocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F45170-B215-4D1B-ADBB-16F1A46BFF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C9B8EB-7D0A-4677-A1C8-77292FEE5E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="6" r:id="rId1"/>
@@ -7698,8 +7698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8221,8 +8221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
confiremd that my sim height, and velocity are very similar. Theta also follows a very similar trend but my sim drops in theta much lower than that of openrocket sim. I must investigate this.
</commit_message>
<xml_diff>
--- a/Barrowman(1.04).xlsx
+++ b/Barrowman(1.04).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bktf3\Desktop\rocket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C9B8EB-7D0A-4677-A1C8-77292FEE5E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7829AD83-0FC6-4589-8E7B-D0DB81110088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="6" r:id="rId1"/>
@@ -7698,7 +7698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
@@ -8221,8 +8221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8350,7 +8350,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="85" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>99</v>
@@ -8446,7 +8446,7 @@
       </c>
       <c r="D12" s="26">
         <f>IF(D8="conical",0.667,IF(D8="parabolic",0.5,IF(D8="ogive", 0.466,0.333)))</f>
-        <v>0.46600000000000003</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="25"/>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="D13" s="28">
         <f>D12*ln</f>
-        <v>74.56</v>
+        <v>80</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>5</v>
@@ -9155,7 +9155,7 @@
       </c>
       <c r="D48" s="47">
         <f>(cnn*xn+cnt*xt+cntb*xtb+cnf*xf)/cnr</f>
-        <v>631.66746652663767</v>
+        <v>632.3220556108173</v>
       </c>
       <c r="E48" s="48" t="s">
         <v>5</v>

</xml_diff>